<commit_message>
updating source numbers in lit_com
</commit_message>
<xml_diff>
--- a/lit_data/litterature NH3 field app digestate.xlsx
+++ b/lit_data/litterature NH3 field app digestate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au583430_uni_au_dk/Documents/Dokumenter/GitHub/Pedersen-2023-app-digestate-NH3-review/lit_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="697" documentId="13_ncr:1_{C1797D30-0D28-4E65-8294-8CCA02D88F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{041A8655-AF25-404D-B1A9-D10C6B5EB71D}"/>
+  <xr:revisionPtr revIDLastSave="754" documentId="13_ncr:1_{C1797D30-0D28-4E65-8294-8CCA02D88F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC9E563B-E008-43D2-976D-52F2A3A33690}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-3045" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{90B750BC-7ABB-4C51-B01A-3142C31660F6}"/>
+    <workbookView xWindow="-38520" yWindow="-3255" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{90B750BC-7ABB-4C51-B01A-3142C31660F6}"/>
   </bookViews>
   <sheets>
     <sheet name="front page" sheetId="1" r:id="rId1"/>
@@ -1843,10 +1843,10 @@
   <dimension ref="A1:AS122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="23" ySplit="2" topLeftCell="X32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="23" ySplit="2" topLeftCell="X54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="S1" sqref="S1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B66" sqref="B66"/>
+      <selection pane="bottomRight" activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7368,7 +7368,7 @@
         <v>28</v>
       </c>
       <c r="B60">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D60" t="s">
         <v>30</v>
@@ -7463,7 +7463,7 @@
         <v>28</v>
       </c>
       <c r="B61">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C61" t="s">
         <v>318</v>
@@ -7576,7 +7576,7 @@
         <v>28</v>
       </c>
       <c r="B62">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D62" t="s">
         <v>30</v>
@@ -7668,7 +7668,7 @@
         <v>28</v>
       </c>
       <c r="B63">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C63" t="s">
         <v>318</v>
@@ -7778,7 +7778,7 @@
         <v>331</v>
       </c>
       <c r="B64">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C64" t="s">
         <v>318</v>
@@ -7882,7 +7882,7 @@
         <v>331</v>
       </c>
       <c r="B65">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C65" t="s">
         <v>318</v>
@@ -7983,7 +7983,7 @@
         <v>331</v>
       </c>
       <c r="B66">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C66" t="s">
         <v>318</v>
@@ -8084,7 +8084,7 @@
         <v>331</v>
       </c>
       <c r="B67">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C67" t="s">
         <v>318</v>
@@ -8188,7 +8188,7 @@
         <v>331</v>
       </c>
       <c r="B68">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C68" t="s">
         <v>318</v>
@@ -8289,7 +8289,7 @@
         <v>331</v>
       </c>
       <c r="B69">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C69" t="s">
         <v>318</v>
@@ -8390,7 +8390,7 @@
         <v>331</v>
       </c>
       <c r="B70">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C70" t="s">
         <v>318</v>
@@ -8494,7 +8494,7 @@
         <v>331</v>
       </c>
       <c r="B71">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C71" t="s">
         <v>318</v>
@@ -8595,7 +8595,7 @@
         <v>331</v>
       </c>
       <c r="B72">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C72" t="s">
         <v>318</v>
@@ -9380,7 +9380,7 @@
         <v>165</v>
       </c>
       <c r="B79" s="15">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D79" s="15" t="s">
         <v>30</v>
@@ -9473,7 +9473,7 @@
         <v>165</v>
       </c>
       <c r="B80" s="15">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C80" s="15" t="s">
         <v>317</v>
@@ -9575,7 +9575,7 @@
         <v>165</v>
       </c>
       <c r="B81" s="15">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D81" s="15" t="s">
         <v>30</v>
@@ -9668,7 +9668,7 @@
         <v>165</v>
       </c>
       <c r="B82" s="15">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C82" s="15" t="s">
         <v>317</v>
@@ -9770,7 +9770,7 @@
         <v>241</v>
       </c>
       <c r="B83">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C83" t="s">
         <v>318</v>
@@ -9860,7 +9860,7 @@
         <v>241</v>
       </c>
       <c r="B84">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C84" t="s">
         <v>318</v>
@@ -9950,7 +9950,7 @@
         <v>241</v>
       </c>
       <c r="B85">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C85" t="s">
         <v>318</v>
@@ -10037,7 +10037,7 @@
         <v>241</v>
       </c>
       <c r="B86">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C86" t="s">
         <v>318</v>
@@ -10130,7 +10130,7 @@
         <v>241</v>
       </c>
       <c r="B87">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C87" t="s">
         <v>318</v>
@@ -10223,7 +10223,7 @@
         <v>241</v>
       </c>
       <c r="B88">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C88" t="s">
         <v>318</v>
@@ -10316,7 +10316,7 @@
         <v>101</v>
       </c>
       <c r="B89">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D89" t="s">
         <v>30</v>
@@ -10408,7 +10408,7 @@
         <v>101</v>
       </c>
       <c r="B90">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C90" t="s">
         <v>318</v>
@@ -10518,7 +10518,7 @@
         <v>101</v>
       </c>
       <c r="B91">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D91" t="s">
         <v>30</v>
@@ -10610,7 +10610,7 @@
         <v>101</v>
       </c>
       <c r="B92">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C92" t="s">
         <v>318</v>
@@ -10720,7 +10720,7 @@
         <v>101</v>
       </c>
       <c r="B93">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D93" t="s">
         <v>30</v>
@@ -10812,7 +10812,7 @@
         <v>101</v>
       </c>
       <c r="B94">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C94" t="s">
         <v>318</v>
@@ -10922,7 +10922,7 @@
         <v>101</v>
       </c>
       <c r="B95">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D95" t="s">
         <v>30</v>
@@ -11014,7 +11014,7 @@
         <v>101</v>
       </c>
       <c r="B96">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C96" t="s">
         <v>318</v>
@@ -11124,7 +11124,7 @@
         <v>133</v>
       </c>
       <c r="B97">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D97" t="s">
         <v>31</v>
@@ -11216,7 +11216,7 @@
         <v>133</v>
       </c>
       <c r="B98">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C98" t="s">
         <v>318</v>
@@ -11329,7 +11329,7 @@
         <v>133</v>
       </c>
       <c r="B99">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C99" t="s">
         <v>318</v>
@@ -11436,7 +11436,7 @@
         <v>133</v>
       </c>
       <c r="B100">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D100" t="s">
         <v>31</v>
@@ -11528,7 +11528,7 @@
         <v>133</v>
       </c>
       <c r="B101">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C101" t="s">
         <v>318</v>
@@ -11641,7 +11641,7 @@
         <v>133</v>
       </c>
       <c r="B102">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C102" t="s">
         <v>318</v>
@@ -11748,7 +11748,7 @@
         <v>145</v>
       </c>
       <c r="B103">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D103" t="s">
         <v>30</v>
@@ -11831,7 +11831,7 @@
         <v>145</v>
       </c>
       <c r="B104">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C104" t="s">
         <v>318</v>
@@ -11921,7 +11921,7 @@
         <v>145</v>
       </c>
       <c r="B105">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C105" t="s">
         <v>318</v>
@@ -12005,7 +12005,7 @@
         <v>145</v>
       </c>
       <c r="B106">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C106" t="s">
         <v>318</v>
@@ -12089,7 +12089,7 @@
         <v>145</v>
       </c>
       <c r="B107">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C107" t="s">
         <v>318</v>
@@ -12173,7 +12173,7 @@
         <v>145</v>
       </c>
       <c r="B108">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C108" t="s">
         <v>318</v>
@@ -12259,7 +12259,7 @@
         <v>145</v>
       </c>
       <c r="B109">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C109" t="s">
         <v>318</v>
@@ -12349,7 +12349,7 @@
         <v>145</v>
       </c>
       <c r="B110">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C110" t="s">
         <v>318</v>
@@ -12433,7 +12433,7 @@
         <v>145</v>
       </c>
       <c r="B111">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C111" t="s">
         <v>318</v>
@@ -12517,7 +12517,7 @@
         <v>145</v>
       </c>
       <c r="B112">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C112" t="s">
         <v>318</v>
@@ -12601,7 +12601,7 @@
         <v>100</v>
       </c>
       <c r="B113">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D113" t="s">
         <v>30</v>
@@ -12687,7 +12687,7 @@
         <v>100</v>
       </c>
       <c r="B114">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C114" t="s">
         <v>318</v>
@@ -12797,7 +12797,7 @@
         <v>100</v>
       </c>
       <c r="B115">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C115" t="s">
         <v>318</v>
@@ -12898,7 +12898,7 @@
         <v>100</v>
       </c>
       <c r="B116">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C116" t="s">
         <v>318</v>
@@ -12999,7 +12999,7 @@
         <v>100</v>
       </c>
       <c r="B117">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C117" t="s">
         <v>318</v>
@@ -13100,7 +13100,7 @@
         <v>100</v>
       </c>
       <c r="B118">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D118" t="s">
         <v>30</v>
@@ -13189,7 +13189,7 @@
         <v>100</v>
       </c>
       <c r="B119">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C119" t="s">
         <v>318</v>
@@ -13299,7 +13299,7 @@
         <v>100</v>
       </c>
       <c r="B120">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C120" t="s">
         <v>318</v>
@@ -13400,7 +13400,7 @@
         <v>100</v>
       </c>
       <c r="B121">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C121" t="s">
         <v>318</v>
@@ -13501,7 +13501,7 @@
         <v>100</v>
       </c>
       <c r="B122">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C122" t="s">
         <v>318</v>

</xml_diff>